<commit_message>
Users import to production #170
</commit_message>
<xml_diff>
--- a/back-end/user_report.xlsx
+++ b/back-end/user_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moayad/Documents/www/risk/back-end/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22205369-BEEB-1443-8721-1FF028FF8801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F66668-0DF9-7D47-9B5B-DDEDE11740D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6600" yWindow="1420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,9 +91,6 @@
     <t>Quinn</t>
   </si>
   <si>
-    <t>Lead</t>
-  </si>
-  <si>
     <t>n.jacob@cgiar.org</t>
   </si>
   <si>
@@ -1412,6 +1409,9 @@
   </si>
   <si>
     <t>Georgios</t>
+  </si>
+  <si>
+    <t>Leader</t>
   </si>
 </sst>
 </file>
@@ -1489,17 +1489,7 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1859,7 +1849,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1949,7 +1939,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1960,13 +1950,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1977,19 +1967,19 @@
         <v>481</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1997,16 +1987,16 @@
         <v>629</v>
       </c>
       <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -2017,16 +2007,16 @@
         <v>81</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -2037,16 +2027,16 @@
         <v>308</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -2057,19 +2047,19 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2077,16 +2067,16 @@
         <v>332</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -2097,16 +2087,16 @@
         <v>601</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2117,19 +2107,19 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2137,16 +2127,16 @@
         <v>297</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -2157,19 +2147,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
         <v>55</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>57</v>
       </c>
-      <c r="E15" t="s">
-        <v>58</v>
-      </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2177,16 +2167,16 @@
         <v>331</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>63</v>
-      </c>
-      <c r="E16" t="s">
-        <v>64</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
@@ -2197,16 +2187,16 @@
         <v>605</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>60</v>
-      </c>
-      <c r="E17" t="s">
-        <v>61</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
@@ -2217,19 +2207,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>66</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>67</v>
       </c>
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2237,16 +2227,16 @@
         <v>267</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
         <v>69</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>70</v>
-      </c>
-      <c r="E19" t="s">
-        <v>71</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -2257,19 +2247,19 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
         <v>72</v>
       </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" t="s">
-        <v>73</v>
-      </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2277,16 +2267,16 @@
         <v>270</v>
       </c>
       <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
         <v>74</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>75</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>76</v>
-      </c>
-      <c r="E21" t="s">
-        <v>77</v>
       </c>
       <c r="F21" t="s">
         <v>10</v>
@@ -2297,19 +2287,19 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
         <v>78</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="s">
-        <v>80</v>
-      </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2317,19 +2307,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2337,16 +2327,16 @@
         <v>140</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
         <v>83</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>84</v>
-      </c>
-      <c r="E24" t="s">
-        <v>85</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
@@ -2357,19 +2347,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
         <v>86</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>87</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>88</v>
       </c>
-      <c r="E25" t="s">
-        <v>89</v>
-      </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2377,16 +2367,16 @@
         <v>272</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
         <v>90</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>91</v>
-      </c>
-      <c r="E26" t="s">
-        <v>92</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
@@ -2397,16 +2387,16 @@
         <v>143</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
         <v>93</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>94</v>
-      </c>
-      <c r="E27" t="s">
-        <v>95</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
@@ -2417,19 +2407,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
         <v>96</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>97</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>98</v>
       </c>
-      <c r="E28" t="s">
-        <v>99</v>
-      </c>
       <c r="F28" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2437,16 +2427,16 @@
         <v>282</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
         <v>100</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>101</v>
-      </c>
-      <c r="E29" t="s">
-        <v>102</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
@@ -2457,19 +2447,19 @@
         <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
         <v>103</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>104</v>
       </c>
-      <c r="E30" t="s">
-        <v>105</v>
-      </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2477,16 +2467,16 @@
         <v>333</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" t="s">
         <v>106</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>107</v>
-      </c>
-      <c r="E31" t="s">
-        <v>108</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
@@ -2497,16 +2487,16 @@
         <v>147</v>
       </c>
       <c r="B32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" t="s">
         <v>109</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>110</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>111</v>
-      </c>
-      <c r="E32" t="s">
-        <v>112</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -2517,16 +2507,16 @@
         <v>574</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" t="s">
         <v>113</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>114</v>
-      </c>
-      <c r="E33" t="s">
-        <v>115</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
@@ -2537,19 +2527,19 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
         <v>116</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>117</v>
       </c>
-      <c r="E34" t="s">
-        <v>118</v>
-      </c>
       <c r="F34" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2557,16 +2547,16 @@
         <v>573</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" t="s">
         <v>119</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>120</v>
-      </c>
-      <c r="E35" t="s">
-        <v>121</v>
       </c>
       <c r="F35" t="s">
         <v>10</v>
@@ -2577,16 +2567,16 @@
         <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
         <v>122</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>123</v>
-      </c>
-      <c r="E36" t="s">
-        <v>124</v>
       </c>
       <c r="F36" t="s">
         <v>10</v>
@@ -2597,19 +2587,19 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" t="s">
         <v>125</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>126</v>
       </c>
-      <c r="E37" t="s">
-        <v>127</v>
-      </c>
       <c r="F37" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2617,16 +2607,16 @@
         <v>148</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" t="s">
         <v>128</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>129</v>
-      </c>
-      <c r="E38" t="s">
-        <v>130</v>
       </c>
       <c r="F38" t="s">
         <v>10</v>
@@ -2637,16 +2627,16 @@
         <v>335</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" t="s">
         <v>131</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>132</v>
-      </c>
-      <c r="E39" t="s">
-        <v>133</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
@@ -2657,16 +2647,16 @@
         <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" t="s">
         <v>134</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>135</v>
-      </c>
-      <c r="E40" t="s">
-        <v>136</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
@@ -2677,16 +2667,16 @@
         <v>151</v>
       </c>
       <c r="B41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" t="s">
         <v>137</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>138</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>139</v>
-      </c>
-      <c r="E41" t="s">
-        <v>140</v>
       </c>
       <c r="F41" t="s">
         <v>10</v>
@@ -2697,19 +2687,19 @@
         <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" t="s">
         <v>141</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>142</v>
       </c>
-      <c r="E42" t="s">
-        <v>143</v>
-      </c>
       <c r="F42" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2717,16 +2707,16 @@
         <v>257</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" t="s">
         <v>144</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>145</v>
-      </c>
-      <c r="E43" t="s">
-        <v>146</v>
       </c>
       <c r="F43" t="s">
         <v>10</v>
@@ -2737,19 +2727,19 @@
         <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
+        <v>146</v>
+      </c>
+      <c r="D44" t="s">
         <v>147</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>148</v>
       </c>
-      <c r="E44" t="s">
-        <v>149</v>
-      </c>
       <c r="F44" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2757,16 +2747,16 @@
         <v>311</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C45" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" t="s">
         <v>150</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>151</v>
-      </c>
-      <c r="E45" t="s">
-        <v>152</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
@@ -2777,19 +2767,19 @@
         <v>154</v>
       </c>
       <c r="B46" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s">
         <v>153</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>154</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>155</v>
       </c>
-      <c r="E46" t="s">
-        <v>156</v>
-      </c>
       <c r="F46" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2797,19 +2787,19 @@
         <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C47" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" t="s">
         <v>157</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>158</v>
       </c>
-      <c r="E47" t="s">
-        <v>159</v>
-      </c>
       <c r="F47" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2817,16 +2807,16 @@
         <v>264</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C48" t="s">
+        <v>159</v>
+      </c>
+      <c r="D48" t="s">
         <v>160</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>161</v>
-      </c>
-      <c r="E48" t="s">
-        <v>162</v>
       </c>
       <c r="F48" t="s">
         <v>10</v>
@@ -2837,16 +2827,16 @@
         <v>594</v>
       </c>
       <c r="B49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" t="s">
         <v>163</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>164</v>
-      </c>
-      <c r="E49" t="s">
-        <v>165</v>
       </c>
       <c r="F49" t="s">
         <v>10</v>
@@ -2857,16 +2847,16 @@
         <v>336</v>
       </c>
       <c r="B50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C50" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" t="s">
         <v>166</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>167</v>
-      </c>
-      <c r="E50" t="s">
-        <v>168</v>
       </c>
       <c r="F50" t="s">
         <v>10</v>
@@ -2877,16 +2867,16 @@
         <v>337</v>
       </c>
       <c r="B51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" t="s">
         <v>169</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>170</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>171</v>
-      </c>
-      <c r="E51" t="s">
-        <v>172</v>
       </c>
       <c r="F51" t="s">
         <v>10</v>
@@ -2897,16 +2887,16 @@
         <v>340</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" t="s">
         <v>173</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>174</v>
-      </c>
-      <c r="E52" t="s">
-        <v>175</v>
       </c>
       <c r="F52" t="s">
         <v>10</v>
@@ -2917,19 +2907,19 @@
         <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C53" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" t="s">
         <v>176</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>177</v>
       </c>
-      <c r="E53" t="s">
-        <v>178</v>
-      </c>
       <c r="F53" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2937,19 +2927,19 @@
         <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C54" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" t="s">
         <v>179</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>180</v>
       </c>
-      <c r="E54" t="s">
-        <v>181</v>
-      </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2957,16 +2947,16 @@
         <v>466</v>
       </c>
       <c r="B55" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" t="s">
         <v>182</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>183</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>184</v>
-      </c>
-      <c r="E55" t="s">
-        <v>185</v>
       </c>
       <c r="F55" t="s">
         <v>10</v>
@@ -2977,16 +2967,16 @@
         <v>36</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C56" t="s">
+        <v>185</v>
+      </c>
+      <c r="D56" t="s">
         <v>186</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>187</v>
-      </c>
-      <c r="E56" t="s">
-        <v>188</v>
       </c>
       <c r="F56" t="s">
         <v>10</v>
@@ -2997,16 +2987,16 @@
         <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C57" t="s">
+        <v>188</v>
+      </c>
+      <c r="D57" t="s">
         <v>189</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>190</v>
-      </c>
-      <c r="E57" t="s">
-        <v>191</v>
       </c>
       <c r="F57" t="s">
         <v>10</v>
@@ -3017,16 +3007,16 @@
         <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C58" t="s">
+        <v>191</v>
+      </c>
+      <c r="D58" t="s">
         <v>192</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>193</v>
-      </c>
-      <c r="E58" t="s">
-        <v>194</v>
       </c>
       <c r="F58" t="s">
         <v>10</v>
@@ -3037,19 +3027,19 @@
         <v>38</v>
       </c>
       <c r="B59" t="s">
+        <v>194</v>
+      </c>
+      <c r="C59" t="s">
         <v>195</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>196</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>197</v>
       </c>
-      <c r="E59" t="s">
-        <v>198</v>
-      </c>
       <c r="F59" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -3057,16 +3047,16 @@
         <v>297</v>
       </c>
       <c r="B60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C60" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" t="s">
         <v>52</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>53</v>
-      </c>
-      <c r="E60" t="s">
-        <v>54</v>
       </c>
       <c r="F60" t="s">
         <v>10</v>
@@ -3077,16 +3067,16 @@
         <v>317</v>
       </c>
       <c r="B61" t="s">
+        <v>198</v>
+      </c>
+      <c r="C61" t="s">
         <v>199</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>200</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>201</v>
-      </c>
-      <c r="E61" t="s">
-        <v>202</v>
       </c>
       <c r="F61" t="s">
         <v>10</v>
@@ -3097,16 +3087,16 @@
         <v>171</v>
       </c>
       <c r="B62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C62" t="s">
+        <v>202</v>
+      </c>
+      <c r="D62" t="s">
         <v>203</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>204</v>
-      </c>
-      <c r="E62" t="s">
-        <v>205</v>
       </c>
       <c r="F62" t="s">
         <v>10</v>
@@ -3117,19 +3107,19 @@
         <v>107</v>
       </c>
       <c r="B63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C63" t="s">
+        <v>205</v>
+      </c>
+      <c r="D63" t="s">
         <v>206</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>207</v>
       </c>
-      <c r="E63" t="s">
-        <v>208</v>
-      </c>
       <c r="F63" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3137,16 +3127,16 @@
         <v>237</v>
       </c>
       <c r="B64" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" t="s">
         <v>209</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>210</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>211</v>
-      </c>
-      <c r="E64" t="s">
-        <v>212</v>
       </c>
       <c r="F64" t="s">
         <v>10</v>
@@ -3157,16 +3147,16 @@
         <v>234</v>
       </c>
       <c r="B65" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C65" t="s">
+        <v>212</v>
+      </c>
+      <c r="D65" t="s">
         <v>213</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>214</v>
-      </c>
-      <c r="E65" t="s">
-        <v>215</v>
       </c>
       <c r="F65" t="s">
         <v>10</v>
@@ -3177,16 +3167,16 @@
         <v>300</v>
       </c>
       <c r="B66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C66" t="s">
+        <v>215</v>
+      </c>
+      <c r="D66" t="s">
         <v>216</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>217</v>
-      </c>
-      <c r="E66" t="s">
-        <v>218</v>
       </c>
       <c r="F66" t="s">
         <v>10</v>
@@ -3197,16 +3187,16 @@
         <v>233</v>
       </c>
       <c r="B67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C67" t="s">
+        <v>218</v>
+      </c>
+      <c r="D67" t="s">
         <v>219</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>220</v>
-      </c>
-      <c r="E67" t="s">
-        <v>221</v>
       </c>
       <c r="F67" t="s">
         <v>10</v>
@@ -3217,16 +3207,16 @@
         <v>236</v>
       </c>
       <c r="B68" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C68" t="s">
+        <v>221</v>
+      </c>
+      <c r="D68" t="s">
         <v>222</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>223</v>
-      </c>
-      <c r="E68" t="s">
-        <v>224</v>
       </c>
       <c r="F68" t="s">
         <v>10</v>
@@ -3237,16 +3227,16 @@
         <v>467</v>
       </c>
       <c r="B69" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C69" t="s">
+        <v>224</v>
+      </c>
+      <c r="D69" t="s">
         <v>225</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>226</v>
-      </c>
-      <c r="E69" t="s">
-        <v>227</v>
       </c>
       <c r="F69" t="s">
         <v>10</v>
@@ -3257,16 +3247,16 @@
         <v>411</v>
       </c>
       <c r="B70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C70" t="s">
+        <v>227</v>
+      </c>
+      <c r="D70" t="s">
         <v>228</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>229</v>
-      </c>
-      <c r="E70" t="s">
-        <v>230</v>
       </c>
       <c r="F70" t="s">
         <v>10</v>
@@ -3277,16 +3267,16 @@
         <v>475</v>
       </c>
       <c r="B71" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C71" t="s">
+        <v>230</v>
+      </c>
+      <c r="D71" t="s">
         <v>231</v>
       </c>
-      <c r="D71" t="s">
-        <v>232</v>
-      </c>
       <c r="E71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F71" t="s">
         <v>10</v>
@@ -3297,19 +3287,19 @@
         <v>43</v>
       </c>
       <c r="B72" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C72" t="s">
+        <v>232</v>
+      </c>
+      <c r="D72" t="s">
         <v>233</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>234</v>
       </c>
-      <c r="E72" t="s">
-        <v>235</v>
-      </c>
       <c r="F72" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -3317,16 +3307,16 @@
         <v>241</v>
       </c>
       <c r="B73" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C73" t="s">
+        <v>235</v>
+      </c>
+      <c r="D73" t="s">
         <v>236</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>237</v>
-      </c>
-      <c r="E73" t="s">
-        <v>238</v>
       </c>
       <c r="F73" t="s">
         <v>10</v>
@@ -3337,16 +3327,16 @@
         <v>240</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C74" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" t="s">
         <v>239</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>240</v>
-      </c>
-      <c r="E74" t="s">
-        <v>241</v>
       </c>
       <c r="F74" t="s">
         <v>10</v>
@@ -3357,16 +3347,16 @@
         <v>474</v>
       </c>
       <c r="B75" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C75" t="s">
+        <v>241</v>
+      </c>
+      <c r="D75" t="s">
         <v>242</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>243</v>
-      </c>
-      <c r="E75" t="s">
-        <v>244</v>
       </c>
       <c r="F75" t="s">
         <v>10</v>
@@ -3377,19 +3367,19 @@
         <v>42</v>
       </c>
       <c r="B76" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C76" t="s">
+        <v>244</v>
+      </c>
+      <c r="D76" t="s">
         <v>245</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>246</v>
       </c>
-      <c r="E76" t="s">
-        <v>247</v>
-      </c>
       <c r="F76" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -3397,16 +3387,16 @@
         <v>472</v>
       </c>
       <c r="B77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C77" t="s">
+        <v>247</v>
+      </c>
+      <c r="D77" t="s">
         <v>248</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>249</v>
-      </c>
-      <c r="E77" t="s">
-        <v>250</v>
       </c>
       <c r="F77" t="s">
         <v>10</v>
@@ -3417,16 +3407,16 @@
         <v>313</v>
       </c>
       <c r="B78" t="s">
+        <v>250</v>
+      </c>
+      <c r="C78" t="s">
         <v>251</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>252</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>253</v>
-      </c>
-      <c r="E78" t="s">
-        <v>254</v>
       </c>
       <c r="F78" t="s">
         <v>10</v>
@@ -3437,19 +3427,19 @@
         <v>45</v>
       </c>
       <c r="B79" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C79" t="s">
+        <v>254</v>
+      </c>
+      <c r="D79" t="s">
         <v>255</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>256</v>
       </c>
-      <c r="E79" t="s">
-        <v>257</v>
-      </c>
       <c r="F79" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -3457,19 +3447,19 @@
         <v>44</v>
       </c>
       <c r="B80" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C80" t="s">
+        <v>257</v>
+      </c>
+      <c r="D80" t="s">
         <v>258</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>259</v>
       </c>
-      <c r="E80" t="s">
-        <v>260</v>
-      </c>
       <c r="F80" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -3477,16 +3467,16 @@
         <v>465</v>
       </c>
       <c r="B81" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C81" t="s">
+        <v>24</v>
+      </c>
+      <c r="D81" t="s">
         <v>25</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>26</v>
-      </c>
-      <c r="E81" t="s">
-        <v>27</v>
       </c>
       <c r="F81" t="s">
         <v>10</v>
@@ -3497,16 +3487,16 @@
         <v>289</v>
       </c>
       <c r="B82" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C82" t="s">
+        <v>260</v>
+      </c>
+      <c r="D82" t="s">
         <v>261</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>262</v>
-      </c>
-      <c r="E82" t="s">
-        <v>263</v>
       </c>
       <c r="F82" t="s">
         <v>10</v>
@@ -3517,16 +3507,16 @@
         <v>489</v>
       </c>
       <c r="B83" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C83" t="s">
+        <v>263</v>
+      </c>
+      <c r="D83" t="s">
         <v>264</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>265</v>
-      </c>
-      <c r="E83" t="s">
-        <v>266</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -3537,19 +3527,19 @@
         <v>177</v>
       </c>
       <c r="B84" t="s">
+        <v>266</v>
+      </c>
+      <c r="C84" t="s">
         <v>267</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>268</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>269</v>
       </c>
-      <c r="E84" t="s">
-        <v>270</v>
-      </c>
       <c r="F84" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -3557,16 +3547,16 @@
         <v>284</v>
       </c>
       <c r="B85" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C85" t="s">
+        <v>270</v>
+      </c>
+      <c r="D85" t="s">
         <v>271</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>272</v>
-      </c>
-      <c r="E85" t="s">
-        <v>273</v>
       </c>
       <c r="F85" t="s">
         <v>10</v>
@@ -3577,16 +3567,16 @@
         <v>178</v>
       </c>
       <c r="B86" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C86" t="s">
+        <v>273</v>
+      </c>
+      <c r="D86" t="s">
         <v>274</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>275</v>
-      </c>
-      <c r="E86" t="s">
-        <v>276</v>
       </c>
       <c r="F86" t="s">
         <v>10</v>
@@ -3597,16 +3587,16 @@
         <v>47</v>
       </c>
       <c r="B87" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C87" t="s">
+        <v>276</v>
+      </c>
+      <c r="D87" t="s">
         <v>277</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>278</v>
-      </c>
-      <c r="E87" t="s">
-        <v>279</v>
       </c>
       <c r="F87" t="s">
         <v>10</v>
@@ -3617,19 +3607,19 @@
         <v>48</v>
       </c>
       <c r="B88" t="s">
+        <v>279</v>
+      </c>
+      <c r="C88" t="s">
         <v>280</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>281</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>282</v>
       </c>
-      <c r="E88" t="s">
-        <v>283</v>
-      </c>
       <c r="F88" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -3637,16 +3627,16 @@
         <v>251</v>
       </c>
       <c r="B89" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C89" t="s">
+        <v>283</v>
+      </c>
+      <c r="D89" t="s">
         <v>284</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>285</v>
-      </c>
-      <c r="E89" t="s">
-        <v>286</v>
       </c>
       <c r="F89" t="s">
         <v>10</v>
@@ -3657,19 +3647,19 @@
         <v>49</v>
       </c>
       <c r="B90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C90" t="s">
+        <v>286</v>
+      </c>
+      <c r="D90" t="s">
         <v>287</v>
       </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>288</v>
       </c>
-      <c r="E90" t="s">
-        <v>289</v>
-      </c>
       <c r="F90" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -3677,16 +3667,16 @@
         <v>185</v>
       </c>
       <c r="B91" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C91" t="s">
+        <v>289</v>
+      </c>
+      <c r="D91" t="s">
         <v>290</v>
       </c>
-      <c r="D91" t="s">
-        <v>291</v>
-      </c>
       <c r="E91" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F91" t="s">
         <v>10</v>
@@ -3697,16 +3687,16 @@
         <v>254</v>
       </c>
       <c r="B92" t="s">
+        <v>291</v>
+      </c>
+      <c r="C92" t="s">
         <v>292</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>293</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>294</v>
-      </c>
-      <c r="E92" t="s">
-        <v>295</v>
       </c>
       <c r="F92" t="s">
         <v>10</v>
@@ -3717,19 +3707,19 @@
         <v>51</v>
       </c>
       <c r="B93" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C93" t="s">
+        <v>295</v>
+      </c>
+      <c r="D93" t="s">
         <v>296</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>297</v>
       </c>
-      <c r="E93" t="s">
-        <v>298</v>
-      </c>
       <c r="F93" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -3737,16 +3727,16 @@
         <v>451</v>
       </c>
       <c r="B94" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C94" t="s">
+        <v>298</v>
+      </c>
+      <c r="D94" t="s">
         <v>299</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>300</v>
-      </c>
-      <c r="E94" t="s">
-        <v>301</v>
       </c>
       <c r="F94" t="s">
         <v>10</v>
@@ -3757,19 +3747,19 @@
         <v>50</v>
       </c>
       <c r="B95" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C95" t="s">
+        <v>301</v>
+      </c>
+      <c r="D95" t="s">
         <v>302</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>303</v>
       </c>
-      <c r="E95" t="s">
-        <v>304</v>
-      </c>
       <c r="F95" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -3777,16 +3767,16 @@
         <v>187</v>
       </c>
       <c r="B96" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C96" t="s">
+        <v>304</v>
+      </c>
+      <c r="D96" t="s">
         <v>305</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>306</v>
-      </c>
-      <c r="E96" t="s">
-        <v>307</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
@@ -3797,16 +3787,16 @@
         <v>117</v>
       </c>
       <c r="B97" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C97" t="s">
+        <v>307</v>
+      </c>
+      <c r="D97" t="s">
         <v>308</v>
       </c>
-      <c r="D97" t="s">
-        <v>309</v>
-      </c>
       <c r="E97" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F97" t="s">
         <v>10</v>
@@ -3817,16 +3807,16 @@
         <v>188</v>
       </c>
       <c r="B98" t="s">
+        <v>309</v>
+      </c>
+      <c r="C98" t="s">
         <v>310</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>311</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>312</v>
-      </c>
-      <c r="E98" t="s">
-        <v>313</v>
       </c>
       <c r="F98" t="s">
         <v>10</v>
@@ -3837,16 +3827,16 @@
         <v>338</v>
       </c>
       <c r="B99" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C99" t="s">
+        <v>313</v>
+      </c>
+      <c r="D99" t="s">
+        <v>97</v>
+      </c>
+      <c r="E99" t="s">
         <v>314</v>
-      </c>
-      <c r="D99" t="s">
-        <v>98</v>
-      </c>
-      <c r="E99" t="s">
-        <v>315</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -3857,19 +3847,19 @@
         <v>52</v>
       </c>
       <c r="B100" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C100" t="s">
+        <v>315</v>
+      </c>
+      <c r="D100" t="s">
         <v>316</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>317</v>
       </c>
-      <c r="E100" t="s">
-        <v>318</v>
-      </c>
       <c r="F100" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -3877,19 +3867,19 @@
         <v>612</v>
       </c>
       <c r="B101" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C101" t="s">
+        <v>318</v>
+      </c>
+      <c r="D101" t="s">
         <v>319</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>320</v>
       </c>
-      <c r="E101" t="s">
-        <v>321</v>
-      </c>
       <c r="F101" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -3897,16 +3887,16 @@
         <v>187</v>
       </c>
       <c r="B102" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C102" t="s">
+        <v>304</v>
+      </c>
+      <c r="D102" t="s">
         <v>305</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>306</v>
-      </c>
-      <c r="E102" t="s">
-        <v>307</v>
       </c>
       <c r="F102" t="s">
         <v>10</v>
@@ -3917,16 +3907,16 @@
         <v>55</v>
       </c>
       <c r="B103" t="s">
+        <v>321</v>
+      </c>
+      <c r="C103" t="s">
         <v>322</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>323</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>324</v>
-      </c>
-      <c r="E103" t="s">
-        <v>325</v>
       </c>
       <c r="F103" t="s">
         <v>10</v>
@@ -3937,19 +3927,19 @@
         <v>342</v>
       </c>
       <c r="B104" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C104" t="s">
+        <v>325</v>
+      </c>
+      <c r="D104" t="s">
         <v>326</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" t="s">
         <v>327</v>
       </c>
-      <c r="E104" t="s">
-        <v>328</v>
-      </c>
       <c r="F104" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -3957,16 +3947,16 @@
         <v>538</v>
       </c>
       <c r="B105" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C105" t="s">
+        <v>328</v>
+      </c>
+      <c r="D105" t="s">
         <v>329</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>330</v>
-      </c>
-      <c r="E105" t="s">
-        <v>331</v>
       </c>
       <c r="F105" t="s">
         <v>10</v>
@@ -3977,16 +3967,16 @@
         <v>451</v>
       </c>
       <c r="B106" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C106" t="s">
+        <v>298</v>
+      </c>
+      <c r="D106" t="s">
         <v>299</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" t="s">
         <v>300</v>
-      </c>
-      <c r="E106" t="s">
-        <v>301</v>
       </c>
       <c r="F106" t="s">
         <v>10</v>
@@ -3997,19 +3987,19 @@
         <v>54</v>
       </c>
       <c r="B107" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C107" t="s">
+        <v>331</v>
+      </c>
+      <c r="D107" t="s">
         <v>332</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>333</v>
       </c>
-      <c r="E107" t="s">
-        <v>334</v>
-      </c>
       <c r="F107" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -4017,16 +4007,16 @@
         <v>341</v>
       </c>
       <c r="B108" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C108" t="s">
+        <v>334</v>
+      </c>
+      <c r="D108" t="s">
         <v>335</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" t="s">
         <v>336</v>
-      </c>
-      <c r="E108" t="s">
-        <v>337</v>
       </c>
       <c r="F108" t="s">
         <v>10</v>
@@ -4037,19 +4027,19 @@
         <v>196</v>
       </c>
       <c r="B109" t="s">
+        <v>337</v>
+      </c>
+      <c r="C109" t="s">
         <v>338</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>339</v>
       </c>
-      <c r="D109" t="s">
+      <c r="E109" t="s">
         <v>340</v>
       </c>
-      <c r="E109" t="s">
-        <v>341</v>
-      </c>
       <c r="F109" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -4057,16 +4047,16 @@
         <v>197</v>
       </c>
       <c r="B110" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C110" t="s">
+        <v>341</v>
+      </c>
+      <c r="D110" t="s">
         <v>342</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
         <v>343</v>
-      </c>
-      <c r="E110" t="s">
-        <v>344</v>
       </c>
       <c r="F110" t="s">
         <v>10</v>
@@ -4077,19 +4067,19 @@
         <v>59</v>
       </c>
       <c r="B111" t="s">
+        <v>344</v>
+      </c>
+      <c r="C111" t="s">
         <v>345</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>346</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
         <v>347</v>
       </c>
-      <c r="E111" t="s">
-        <v>348</v>
-      </c>
       <c r="F111" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -4097,16 +4087,16 @@
         <v>198</v>
       </c>
       <c r="B112" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C112" t="s">
+        <v>348</v>
+      </c>
+      <c r="D112" t="s">
         <v>349</v>
       </c>
-      <c r="D112" t="s">
+      <c r="E112" t="s">
         <v>350</v>
-      </c>
-      <c r="E112" t="s">
-        <v>351</v>
       </c>
       <c r="F112" t="s">
         <v>10</v>
@@ -4117,16 +4107,16 @@
         <v>465</v>
       </c>
       <c r="B113" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C113" t="s">
+        <v>24</v>
+      </c>
+      <c r="D113" t="s">
         <v>25</v>
       </c>
-      <c r="D113" t="s">
+      <c r="E113" t="s">
         <v>26</v>
-      </c>
-      <c r="E113" t="s">
-        <v>27</v>
       </c>
       <c r="F113" t="s">
         <v>10</v>
@@ -4137,19 +4127,19 @@
         <v>65</v>
       </c>
       <c r="B114" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C114" t="s">
+        <v>351</v>
+      </c>
+      <c r="D114" t="s">
         <v>352</v>
       </c>
-      <c r="D114" t="s">
+      <c r="E114" t="s">
         <v>353</v>
       </c>
-      <c r="E114" t="s">
-        <v>354</v>
-      </c>
       <c r="F114" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -4157,16 +4147,16 @@
         <v>339</v>
       </c>
       <c r="B115" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C115" t="s">
+        <v>354</v>
+      </c>
+      <c r="D115" t="s">
         <v>355</v>
       </c>
-      <c r="D115" t="s">
+      <c r="E115" t="s">
         <v>356</v>
-      </c>
-      <c r="E115" t="s">
-        <v>357</v>
       </c>
       <c r="F115" t="s">
         <v>10</v>
@@ -4177,19 +4167,19 @@
         <v>569</v>
       </c>
       <c r="B116" t="s">
+        <v>357</v>
+      </c>
+      <c r="C116" t="s">
         <v>358</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>359</v>
       </c>
-      <c r="D116" t="s">
+      <c r="E116" t="s">
         <v>360</v>
       </c>
-      <c r="E116" t="s">
-        <v>361</v>
-      </c>
       <c r="F116" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -4197,16 +4187,16 @@
         <v>633</v>
       </c>
       <c r="B117" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C117" t="s">
+        <v>361</v>
+      </c>
+      <c r="D117" t="s">
         <v>362</v>
       </c>
-      <c r="D117" t="s">
+      <c r="E117" t="s">
         <v>363</v>
-      </c>
-      <c r="E117" t="s">
-        <v>364</v>
       </c>
       <c r="F117" t="s">
         <v>10</v>
@@ -4217,19 +4207,19 @@
         <v>60</v>
       </c>
       <c r="B118" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C118" t="s">
+        <v>364</v>
+      </c>
+      <c r="D118" t="s">
         <v>365</v>
       </c>
-      <c r="D118" t="s">
+      <c r="E118" t="s">
         <v>366</v>
       </c>
-      <c r="E118" t="s">
-        <v>367</v>
-      </c>
       <c r="F118" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -4237,16 +4227,16 @@
         <v>205</v>
       </c>
       <c r="B119" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C119" t="s">
+        <v>367</v>
+      </c>
+      <c r="D119" t="s">
         <v>368</v>
       </c>
-      <c r="D119" t="s">
+      <c r="E119" t="s">
         <v>369</v>
-      </c>
-      <c r="E119" t="s">
-        <v>370</v>
       </c>
       <c r="F119" t="s">
         <v>10</v>
@@ -4257,16 +4247,16 @@
         <v>206</v>
       </c>
       <c r="B120" t="s">
+        <v>370</v>
+      </c>
+      <c r="C120" t="s">
         <v>371</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
         <v>372</v>
       </c>
-      <c r="D120" t="s">
+      <c r="E120" t="s">
         <v>373</v>
-      </c>
-      <c r="E120" t="s">
-        <v>374</v>
       </c>
       <c r="F120" t="s">
         <v>10</v>
@@ -4277,19 +4267,19 @@
         <v>461</v>
       </c>
       <c r="B121" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C121" t="s">
+        <v>374</v>
+      </c>
+      <c r="D121" t="s">
         <v>375</v>
       </c>
-      <c r="D121" t="s">
+      <c r="E121" t="s">
         <v>376</v>
       </c>
-      <c r="E121" t="s">
-        <v>377</v>
-      </c>
       <c r="F121" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -4297,19 +4287,19 @@
         <v>63</v>
       </c>
       <c r="B122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C122" t="s">
+        <v>377</v>
+      </c>
+      <c r="D122" t="s">
         <v>378</v>
       </c>
-      <c r="D122" t="s">
+      <c r="E122" t="s">
         <v>379</v>
       </c>
-      <c r="E122" t="s">
-        <v>380</v>
-      </c>
       <c r="F122" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -4317,19 +4307,19 @@
         <v>295</v>
       </c>
       <c r="B123" t="s">
+        <v>380</v>
+      </c>
+      <c r="C123" t="s">
         <v>381</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
         <v>382</v>
       </c>
-      <c r="D123" t="s">
+      <c r="E123" t="s">
         <v>383</v>
       </c>
-      <c r="E123" t="s">
-        <v>384</v>
-      </c>
       <c r="F123" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -4337,19 +4327,19 @@
         <v>64</v>
       </c>
       <c r="B124" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C124" t="s">
+        <v>384</v>
+      </c>
+      <c r="D124" t="s">
         <v>385</v>
       </c>
-      <c r="D124" t="s">
+      <c r="E124" t="s">
         <v>386</v>
       </c>
-      <c r="E124" t="s">
-        <v>387</v>
-      </c>
       <c r="F124" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -4357,16 +4347,16 @@
         <v>208</v>
       </c>
       <c r="B125" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C125" t="s">
+        <v>387</v>
+      </c>
+      <c r="D125" t="s">
         <v>388</v>
       </c>
-      <c r="D125" t="s">
+      <c r="E125" t="s">
         <v>389</v>
-      </c>
-      <c r="E125" t="s">
-        <v>390</v>
       </c>
       <c r="F125" t="s">
         <v>10</v>
@@ -4377,16 +4367,16 @@
         <v>592</v>
       </c>
       <c r="B126" t="s">
+        <v>390</v>
+      </c>
+      <c r="C126" t="s">
         <v>391</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>392</v>
       </c>
-      <c r="D126" t="s">
+      <c r="E126" t="s">
         <v>393</v>
-      </c>
-      <c r="E126" t="s">
-        <v>394</v>
       </c>
       <c r="F126" t="s">
         <v>10</v>
@@ -4397,16 +4387,16 @@
         <v>257</v>
       </c>
       <c r="B127" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C127" t="s">
+        <v>143</v>
+      </c>
+      <c r="D127" t="s">
         <v>144</v>
       </c>
-      <c r="D127" t="s">
+      <c r="E127" t="s">
         <v>145</v>
-      </c>
-      <c r="E127" t="s">
-        <v>146</v>
       </c>
       <c r="F127" t="s">
         <v>10</v>
@@ -4417,19 +4407,19 @@
         <v>66</v>
       </c>
       <c r="B128" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C128" t="s">
+        <v>394</v>
+      </c>
+      <c r="D128" t="s">
         <v>395</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" t="s">
         <v>396</v>
       </c>
-      <c r="E128" t="s">
-        <v>397</v>
-      </c>
       <c r="F128" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -4437,19 +4427,19 @@
         <v>67</v>
       </c>
       <c r="B129" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C129" t="s">
+        <v>397</v>
+      </c>
+      <c r="D129" t="s">
         <v>398</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E129" t="s">
         <v>399</v>
       </c>
-      <c r="E129" t="s">
-        <v>400</v>
-      </c>
       <c r="F129" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -4457,19 +4447,19 @@
         <v>108</v>
       </c>
       <c r="B130" t="s">
+        <v>400</v>
+      </c>
+      <c r="C130" t="s">
         <v>401</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
         <v>402</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" t="s">
         <v>403</v>
       </c>
-      <c r="E130" t="s">
-        <v>404</v>
-      </c>
       <c r="F130" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -4477,16 +4467,16 @@
         <v>210</v>
       </c>
       <c r="B131" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C131" t="s">
+        <v>404</v>
+      </c>
+      <c r="D131" t="s">
         <v>405</v>
       </c>
-      <c r="D131" t="s">
+      <c r="E131" t="s">
         <v>406</v>
-      </c>
-      <c r="E131" t="s">
-        <v>407</v>
       </c>
       <c r="F131" t="s">
         <v>10</v>
@@ -4497,16 +4487,16 @@
         <v>211</v>
       </c>
       <c r="B132" t="s">
+        <v>407</v>
+      </c>
+      <c r="C132" t="s">
         <v>408</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>409</v>
       </c>
-      <c r="D132" t="s">
+      <c r="E132" t="s">
         <v>410</v>
-      </c>
-      <c r="E132" t="s">
-        <v>411</v>
       </c>
       <c r="F132" t="s">
         <v>10</v>
@@ -4517,16 +4507,16 @@
         <v>600</v>
       </c>
       <c r="B133" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C133" t="s">
+        <v>411</v>
+      </c>
+      <c r="D133" t="s">
         <v>412</v>
       </c>
-      <c r="D133" t="s">
-        <v>413</v>
-      </c>
       <c r="E133" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
@@ -4537,16 +4527,16 @@
         <v>466</v>
       </c>
       <c r="B134" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C134" t="s">
+        <v>182</v>
+      </c>
+      <c r="D134" t="s">
         <v>183</v>
       </c>
-      <c r="D134" t="s">
+      <c r="E134" t="s">
         <v>184</v>
-      </c>
-      <c r="E134" t="s">
-        <v>185</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -4557,19 +4547,19 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C135" t="s">
+        <v>413</v>
+      </c>
+      <c r="D135" t="s">
         <v>414</v>
       </c>
-      <c r="D135" t="s">
+      <c r="E135" t="s">
         <v>415</v>
       </c>
-      <c r="E135" t="s">
-        <v>416</v>
-      </c>
       <c r="F135" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -4577,16 +4567,16 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C136" t="s">
+        <v>416</v>
+      </c>
+      <c r="D136" t="s">
         <v>417</v>
       </c>
-      <c r="D136" t="s">
+      <c r="E136" t="s">
         <v>418</v>
-      </c>
-      <c r="E136" t="s">
-        <v>419</v>
       </c>
       <c r="F136" t="s">
         <v>10</v>
@@ -4597,19 +4587,19 @@
         <v>602</v>
       </c>
       <c r="B137" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C137" t="s">
+        <v>419</v>
+      </c>
+      <c r="D137" t="s">
+        <v>40</v>
+      </c>
+      <c r="E137" t="s">
         <v>420</v>
       </c>
-      <c r="D137" t="s">
-        <v>41</v>
-      </c>
-      <c r="E137" t="s">
-        <v>421</v>
-      </c>
       <c r="F137" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -4617,16 +4607,16 @@
         <v>465</v>
       </c>
       <c r="B138" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C138" t="s">
+        <v>24</v>
+      </c>
+      <c r="D138" t="s">
         <v>25</v>
       </c>
-      <c r="D138" t="s">
+      <c r="E138" t="s">
         <v>26</v>
-      </c>
-      <c r="E138" t="s">
-        <v>27</v>
       </c>
       <c r="F138" t="s">
         <v>10</v>
@@ -4637,16 +4627,16 @@
         <v>115</v>
       </c>
       <c r="B139" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C139" t="s">
+        <v>421</v>
+      </c>
+      <c r="D139" t="s">
         <v>422</v>
       </c>
-      <c r="D139" t="s">
+      <c r="E139" t="s">
         <v>423</v>
-      </c>
-      <c r="E139" t="s">
-        <v>424</v>
       </c>
       <c r="F139" t="s">
         <v>10</v>
@@ -4657,16 +4647,16 @@
         <v>18</v>
       </c>
       <c r="B140" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C140" t="s">
+        <v>424</v>
+      </c>
+      <c r="D140" t="s">
         <v>425</v>
       </c>
-      <c r="D140" t="s">
+      <c r="E140" t="s">
         <v>426</v>
-      </c>
-      <c r="E140" t="s">
-        <v>427</v>
       </c>
       <c r="F140" t="s">
         <v>10</v>
@@ -4677,16 +4667,16 @@
         <v>451</v>
       </c>
       <c r="B141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C141" t="s">
+        <v>298</v>
+      </c>
+      <c r="D141" t="s">
         <v>299</v>
       </c>
-      <c r="D141" t="s">
+      <c r="E141" t="s">
         <v>300</v>
-      </c>
-      <c r="E141" t="s">
-        <v>301</v>
       </c>
       <c r="F141" t="s">
         <v>10</v>
@@ -4697,19 +4687,19 @@
         <v>194</v>
       </c>
       <c r="B142" t="s">
+        <v>427</v>
+      </c>
+      <c r="C142" t="s">
         <v>428</v>
       </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
         <v>429</v>
       </c>
-      <c r="D142" t="s">
+      <c r="E142" t="s">
         <v>430</v>
       </c>
-      <c r="E142" t="s">
-        <v>431</v>
-      </c>
       <c r="F142" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
@@ -4717,16 +4707,16 @@
         <v>179</v>
       </c>
       <c r="B143" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C143" t="s">
+        <v>431</v>
+      </c>
+      <c r="D143" t="s">
         <v>432</v>
       </c>
-      <c r="D143" t="s">
+      <c r="E143" t="s">
         <v>433</v>
-      </c>
-      <c r="E143" t="s">
-        <v>434</v>
       </c>
       <c r="F143" t="s">
         <v>10</v>
@@ -4737,19 +4727,19 @@
         <v>582</v>
       </c>
       <c r="B144" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C144" t="s">
+        <v>434</v>
+      </c>
+      <c r="D144" t="s">
+        <v>150</v>
+      </c>
+      <c r="E144" t="s">
         <v>435</v>
       </c>
-      <c r="D144" t="s">
-        <v>151</v>
-      </c>
-      <c r="E144" t="s">
-        <v>436</v>
-      </c>
       <c r="F144" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -4757,16 +4747,16 @@
         <v>520</v>
       </c>
       <c r="B145" t="s">
+        <v>436</v>
+      </c>
+      <c r="C145" t="s">
         <v>437</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>438</v>
       </c>
-      <c r="D145" t="s">
+      <c r="E145" t="s">
         <v>439</v>
-      </c>
-      <c r="E145" t="s">
-        <v>440</v>
       </c>
       <c r="F145" t="s">
         <v>10</v>
@@ -4777,16 +4767,16 @@
         <v>198</v>
       </c>
       <c r="B146" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C146" t="s">
+        <v>348</v>
+      </c>
+      <c r="D146" t="s">
         <v>349</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" t="s">
         <v>350</v>
-      </c>
-      <c r="E146" t="s">
-        <v>351</v>
       </c>
       <c r="F146" t="s">
         <v>10</v>
@@ -4797,16 +4787,16 @@
         <v>342</v>
       </c>
       <c r="B147" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C147" t="s">
+        <v>325</v>
+      </c>
+      <c r="D147" t="s">
         <v>326</v>
       </c>
-      <c r="D147" t="s">
+      <c r="E147" t="s">
         <v>327</v>
-      </c>
-      <c r="E147" t="s">
-        <v>328</v>
       </c>
       <c r="F147" t="s">
         <v>10</v>
@@ -4817,16 +4807,16 @@
         <v>538</v>
       </c>
       <c r="B148" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C148" t="s">
+        <v>328</v>
+      </c>
+      <c r="D148" t="s">
         <v>329</v>
       </c>
-      <c r="D148" t="s">
+      <c r="E148" t="s">
         <v>330</v>
-      </c>
-      <c r="E148" t="s">
-        <v>331</v>
       </c>
       <c r="F148" t="s">
         <v>10</v>
@@ -4837,16 +4827,16 @@
         <v>343</v>
       </c>
       <c r="B149" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C149" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D149" t="s">
         <v>12</v>
       </c>
       <c r="E149" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F149" t="s">
         <v>10</v>
@@ -4857,19 +4847,19 @@
         <v>54</v>
       </c>
       <c r="B150" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C150" t="s">
+        <v>331</v>
+      </c>
+      <c r="D150" t="s">
         <v>332</v>
       </c>
-      <c r="D150" t="s">
+      <c r="E150" t="s">
         <v>333</v>
       </c>
-      <c r="E150" t="s">
-        <v>334</v>
-      </c>
       <c r="F150" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
@@ -4877,16 +4867,16 @@
         <v>341</v>
       </c>
       <c r="B151" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C151" t="s">
+        <v>334</v>
+      </c>
+      <c r="D151" t="s">
         <v>335</v>
       </c>
-      <c r="D151" t="s">
+      <c r="E151" t="s">
         <v>336</v>
-      </c>
-      <c r="E151" t="s">
-        <v>337</v>
       </c>
       <c r="F151" t="s">
         <v>10</v>
@@ -4897,19 +4887,19 @@
         <v>286</v>
       </c>
       <c r="B152" t="s">
+        <v>442</v>
+      </c>
+      <c r="C152" t="s">
         <v>443</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D152" t="s">
         <v>444</v>
       </c>
-      <c r="D152" t="s">
+      <c r="E152" t="s">
         <v>445</v>
       </c>
-      <c r="E152" t="s">
-        <v>446</v>
-      </c>
       <c r="F152" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
@@ -4917,39 +4907,39 @@
         <v>254</v>
       </c>
       <c r="B153" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C153" t="s">
+        <v>292</v>
+      </c>
+      <c r="D153" t="s">
         <v>293</v>
       </c>
-      <c r="D153" t="s">
+      <c r="E153" t="s">
         <v>294</v>
       </c>
-      <c r="E153" t="s">
-        <v>295</v>
-      </c>
       <c r="F153" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
+        <v>446</v>
+      </c>
+      <c r="B154" t="s">
+        <v>442</v>
+      </c>
+      <c r="C154" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="B154" t="s">
-        <v>443</v>
-      </c>
-      <c r="C154" s="4" t="s">
+      <c r="D154" t="s">
+        <v>456</v>
+      </c>
+      <c r="E154" t="s">
         <v>448</v>
       </c>
-      <c r="D154" t="s">
-        <v>457</v>
-      </c>
-      <c r="E154" t="s">
-        <v>449</v>
-      </c>
       <c r="F154" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -4957,19 +4947,19 @@
         <v>591</v>
       </c>
       <c r="B155" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C155" t="s">
+        <v>449</v>
+      </c>
+      <c r="D155" t="s">
         <v>450</v>
       </c>
-      <c r="D155" t="s">
+      <c r="E155" t="s">
         <v>451</v>
       </c>
-      <c r="E155" t="s">
-        <v>452</v>
-      </c>
       <c r="F155" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -4977,30 +4967,30 @@
         <v>90</v>
       </c>
       <c r="B156" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C156" t="s">
+        <v>452</v>
+      </c>
+      <c r="D156" t="s">
         <v>453</v>
       </c>
-      <c r="D156" t="s">
+      <c r="E156" t="s">
         <v>454</v>
       </c>
-      <c r="E156" t="s">
+      <c r="F156" t="s">
         <v>455</v>
-      </c>
-      <c r="F156" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C183" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C156">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C157:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C156">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C154" r:id="rId1" xr:uid="{ECF37A68-90D5-7142-A04B-BDCC5C28B8E3}"/>

</xml_diff>